<commit_message>
make new directory. split time series data
</commit_message>
<xml_diff>
--- a/results/annotation/AbioticSamples_ATH.xlsx
+++ b/results/annotation/AbioticSamples_ATH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28421"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="765" activeTab="2"/>
+    <workbookView xWindow="3100" yWindow="0" windowWidth="31440" windowHeight="16060" tabRatio="765" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All Samples" sheetId="3" r:id="rId1"/>
@@ -3498,7 +3498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4265,8 +4265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD24"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4432,20 +4432,20 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" s="2" customFormat="1">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -4551,163 +4551,163 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" s="2" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" s="2" customFormat="1">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
         <v>12</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" s="2" customFormat="1">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
         <v>12</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" s="2" customFormat="1">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
         <v>14</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" s="2" customFormat="1">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" s="2" customFormat="1">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
         <v>14</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" s="2" customFormat="1">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
         <v>14</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" s="2" customFormat="1">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="2" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4781,12 +4781,22 @@
   <dimension ref="A1:M209"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="41.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -13125,7 +13135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A112" sqref="A1:XFD112"/>
     </sheetView>
   </sheetViews>

</xml_diff>